<commit_message>
allowed to keep tip in dilute and apply
</commit_message>
<xml_diff>
--- a/protocols/CODEX/labware layout_CODEX_v0.12.xlsx
+++ b/protocols/CODEX/labware layout_CODEX_v0.12.xlsx
@@ -70,7 +70,7 @@
     <t>Omni-Stainer module</t>
   </si>
   <si>
-    <t>C12/S12</t>
+    <t>S12</t>
   </si>
   <si>
     <t>Num samples:</t>
@@ -103,27 +103,27 @@
     <t>Preblock</t>
   </si>
   <si>
+    <t>210 μL</t>
+  </si>
+  <si>
+    <t>Staining buffer without antibodies, but with blocking components N/J/G/S</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Ab cocktail 1</t>
+  </si>
+  <si>
+    <t>Ab cocktail 2</t>
+  </si>
+  <si>
+    <t>Ab cocktail 3</t>
+  </si>
+  <si>
     <t>120 μL</t>
   </si>
   <si>
-    <t>Staining buffer without antibodies, but with blocking components N/J/G/S</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Ab cocktail 1</t>
-  </si>
-  <si>
-    <t>Ab cocktail 2</t>
-  </si>
-  <si>
-    <t>Ab cocktail 3</t>
-  </si>
-  <si>
-    <t>70 μL</t>
-  </si>
-  <si>
     <t>Antibody mix in Staining buffer with blocking components N/J/G/S, as per Akoya instructions</t>
   </si>
   <si>
@@ -133,7 +133,7 @@
     <t>Reagent F</t>
   </si>
   <si>
-    <t>2.5 μL</t>
+    <t>5 μL</t>
   </si>
   <si>
     <t xml:space="preserve">Reagent F aliquots can be safely stored at room temperature for the duration of the protiocol, as long as the plate is sealed with foil immediately after filling </t>
@@ -277,7 +277,7 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>C12/S12</t>
+      <t>S12</t>
     </r>
     <r>
       <rPr>
@@ -3437,7 +3437,7 @@
         <f>IF(M$11&lt;=$D$5,"Preblock","")</f>
       </c>
       <c r="N12" t="s" s="47">
-        <f>IF(FIND("C12",$D$4)&gt;0,120,210)&amp;" μL"</f>
+        <f>IF(_xlfn.IFERROR(FIND("C12",$D$4),0)&gt;0,120,210)&amp;" μL"</f>
         <v>14</v>
       </c>
       <c r="O12" t="s" s="48">
@@ -3494,7 +3494,7 @@
         <f>IF(M$11&lt;=$D$5,"Ab cocktail "&amp;M$11,"")</f>
       </c>
       <c r="N13" t="s" s="47">
-        <f>IF(FIND("C12",$D$4)&gt;0,70,120)&amp;" μL"</f>
+        <f>IF(_xlfn.IFERROR(FIND("C12",$D$4),0)&gt;0,70,120)&amp;" μL"</f>
         <v>20</v>
       </c>
       <c r="O13" t="s" s="48">
@@ -3551,7 +3551,7 @@
         <f>IF(M$11&lt;=$D$5,"Reagent F","")</f>
       </c>
       <c r="N14" t="s" s="47">
-        <f>IF(FIND("C12",$D$4)&gt;0,2.5,5)&amp;" μL"</f>
+        <f>IF(_xlfn.IFERROR(FIND("C12",$D$4),0)&gt;0,2.5,5)&amp;" μL"</f>
         <v>24</v>
       </c>
       <c r="O14" t="s" s="48">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="N15" t="s" s="52">
         <f>IF(D7="No","","120 μL")</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O15" t="s" s="53">
         <f>IF(D7="No","","Detector oligo mix in Screening Buffer with Assay Component ")</f>

</xml_diff>